<commit_message>
updated registration test data for the date column in yyyy-mm-dd format in the excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/registration-test-data.xlsx
+++ b/src/test/resources/registration-test-data.xlsx
@@ -52,7 +52,7 @@
     <t>Freddy</t>
   </si>
   <si>
-    <t>01/04/1987</t>
+    <t>1987-01-04</t>
   </si>
   <si>
     <t>New Dallas Street</t>
@@ -82,7 +82,7 @@
     <t>Roger</t>
   </si>
   <si>
-    <t>07/12/1978</t>
+    <t>1978-07-12</t>
   </si>
   <si>
     <t>Old Traffarod Road</t>
@@ -112,7 +112,7 @@
     <t>Einstein</t>
   </si>
   <si>
-    <t>09/09/1987</t>
+    <t>1987-09-09</t>
   </si>
   <si>
     <t>Hospital Hollow</t>
@@ -139,7 +139,7 @@
     <t>Novel</t>
   </si>
   <si>
-    <t>09/01/1978</t>
+    <t>1978-09-01</t>
   </si>
   <si>
     <t>Ashleigh Banks</t>
@@ -166,7 +166,7 @@
     <t>Benn</t>
   </si>
   <si>
-    <t>19/11/1967</t>
+    <t>1967-11-19</t>
   </si>
   <si>
     <t>Downland Close</t>
@@ -193,7 +193,7 @@
     <t>Cummins</t>
   </si>
   <si>
-    <t>11/12/1974</t>
+    <t>1974-11-12</t>
   </si>
   <si>
     <t>Heol Y Llidiart-Coch</t>
@@ -220,7 +220,7 @@
     <t>Cook</t>
   </si>
   <si>
-    <t>05/06/1975</t>
+    <t>1975-05-06</t>
   </si>
   <si>
     <t>Pump Heights</t>
@@ -247,7 +247,7 @@
     <t>Miller</t>
   </si>
   <si>
-    <t>07/08/1976</t>
+    <t>1976-07-08</t>
   </si>
   <si>
     <t>Yetlands</t>
@@ -274,7 +274,7 @@
     <t>Davis</t>
   </si>
   <si>
-    <t>15/10/1998</t>
+    <t>1998-10-15</t>
   </si>
   <si>
     <t>Thornsett Place</t>
@@ -298,7 +298,7 @@
     <t>Julia</t>
   </si>
   <si>
-    <t>10/12/1989</t>
+    <t>1989-10-12</t>
   </si>
   <si>
     <t>Kay Cottages</t>
@@ -322,7 +322,7 @@
     <t>Anne</t>
   </si>
   <si>
-    <t>14/10/1987</t>
+    <t>1987-10-14</t>
   </si>
   <si>
     <t>Swinley Gardens</t>
@@ -349,7 +349,7 @@
     <t>Jones</t>
   </si>
   <si>
-    <t>05/01/1986</t>
+    <t>1986-05-01</t>
   </si>
   <si>
     <t>Fowler Isaf</t>
@@ -376,7 +376,7 @@
     <t>Johnson</t>
   </si>
   <si>
-    <t>05/07/1986</t>
+    <t>1986-05-07</t>
   </si>
   <si>
     <t>Texas Street</t>
@@ -403,7 +403,7 @@
     <t>Gabba</t>
   </si>
   <si>
-    <t>13/01/1980</t>
+    <t>1980-01-13</t>
   </si>
   <si>
     <t>Old post office street</t>
@@ -430,7 +430,7 @@
     <t>Trump</t>
   </si>
   <si>
-    <t>01/05/1979</t>
+    <t>1979-01-05</t>
   </si>
   <si>
     <t>Trafford Lane</t>
@@ -457,7 +457,7 @@
     <t>Biden</t>
   </si>
   <si>
-    <t>16/11/1999</t>
+    <t>1999-11-16</t>
   </si>
   <si>
     <t>Ruskin street</t>
@@ -484,7 +484,7 @@
     <t>Flair</t>
   </si>
   <si>
-    <t>31/07/1990</t>
+    <t>1990-07-31</t>
   </si>
   <si>
     <t>Classic Street</t>
@@ -511,7 +511,7 @@
     <t>Powell</t>
   </si>
   <si>
-    <t>29/03/1981</t>
+    <t>1981-03-29</t>
   </si>
   <si>
     <t>New Restaurant road</t>
@@ -535,7 +535,7 @@
     <t>Jean</t>
   </si>
   <si>
-    <t>18/02/1984</t>
+    <t>1984-02-18</t>
   </si>
   <si>
     <t>Cafe Coffee Day street</t>
@@ -615,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -623,6 +623,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -633,6 +636,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -902,7 +908,7 @@
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -914,7 +920,7 @@
       <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -937,7 +943,7 @@
       <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -949,7 +955,7 @@
       <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -972,19 +978,19 @@
       <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>37</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1001,28 +1007,28 @@
       <c r="B5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -1036,28 +1042,28 @@
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="8" t="s">
         <v>57</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -1071,28 +1077,28 @@
       <c r="B7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="8" t="s">
         <v>66</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -1106,28 +1112,28 @@
       <c r="B8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>73</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="8" t="s">
         <v>75</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -1141,28 +1147,28 @@
       <c r="B9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>82</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="8" t="s">
         <v>84</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1176,28 +1182,28 @@
       <c r="B10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
         <v>91</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="8" t="s">
         <v>93</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1211,28 +1217,28 @@
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="6" t="s">
         <v>99</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="8" t="s">
         <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1246,28 +1252,28 @@
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>105</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="6" t="s">
         <v>107</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="8" t="s">
         <v>109</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1281,28 +1287,28 @@
       <c r="B13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="7" t="s">
         <v>112</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="4" t="s">
         <v>114</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="6" t="s">
         <v>116</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1316,28 +1322,28 @@
       <c r="B14" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="6" t="s">
         <v>125</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="8" t="s">
         <v>127</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1351,28 +1357,28 @@
       <c r="B15" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="7" t="s">
         <v>130</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="4" t="s">
         <v>132</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="6" t="s">
         <v>134</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="8" t="s">
         <v>136</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -1386,28 +1392,28 @@
       <c r="B16" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="7" t="s">
         <v>139</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>141</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="6" t="s">
         <v>143</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="8" t="s">
         <v>145</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1421,28 +1427,28 @@
       <c r="B17" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="7" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>150</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="6" t="s">
         <v>152</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="8" t="s">
         <v>154</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -1456,28 +1462,28 @@
       <c r="B18" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="7" t="s">
         <v>157</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>159</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="6" t="s">
         <v>161</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="8" t="s">
         <v>163</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1491,28 +1497,28 @@
       <c r="B19" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="7" t="s">
         <v>166</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>168</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="6" t="s">
         <v>46</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="8" t="s">
         <v>171</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -1526,28 +1532,28 @@
       <c r="B20" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="7" t="s">
         <v>174</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>176</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="6" t="s">
         <v>178</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J20" s="8" t="s">
         <v>180</v>
       </c>
       <c r="K20" s="2" t="s">

</xml_diff>